<commit_message>
Création des formulaires pour les maquettes graphiques et modification du fichier excel
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
   <si>
     <t>Type</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Ac.gif</t>
+  </si>
+  <si>
+    <t>Nom</t>
   </si>
 </sst>
 </file>
@@ -483,32 +486,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -516,16 +522,19 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -533,16 +542,19 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -550,16 +562,19 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -567,16 +582,19 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -584,16 +602,19 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -601,16 +622,19 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -618,16 +642,19 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -635,16 +662,19 @@
         <v>5</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -652,16 +682,19 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D10">
         <v>11</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -669,16 +702,19 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -686,16 +722,19 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -703,16 +742,19 @@
         <v>8</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -720,16 +762,19 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
         <v>14</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -737,16 +782,19 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>10</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -754,16 +802,19 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
         <v>20</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -771,16 +822,19 @@
         <v>4</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D17">
         <v>3</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -788,16 +842,19 @@
         <v>5</v>
       </c>
       <c r="C18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -805,16 +862,19 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19">
         <v>11</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -822,16 +882,19 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -839,16 +902,19 @@
         <v>7</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -856,16 +922,19 @@
         <v>8</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -873,16 +942,19 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
         <v>14</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -890,16 +962,19 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>10</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -907,16 +982,19 @@
         <v>3</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
         <v>20</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -924,16 +1002,19 @@
         <v>4</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D26">
         <v>3</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -941,16 +1022,19 @@
         <v>5</v>
       </c>
       <c r="C27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D27">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -958,16 +1042,19 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <v>11</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28">
+        <v>11</v>
+      </c>
+      <c r="F28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -975,16 +1062,19 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -992,16 +1082,19 @@
         <v>7</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1009,16 +1102,19 @@
         <v>8</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1026,16 +1122,19 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
         <v>14</v>
       </c>
-      <c r="E32" t="s">
+      <c r="F32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1043,16 +1142,19 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>10</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1060,16 +1162,19 @@
         <v>3</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
         <v>20</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1077,16 +1182,19 @@
         <v>4</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D35">
         <v>3</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35">
+        <v>3</v>
+      </c>
+      <c r="F35" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1094,16 +1202,19 @@
         <v>5</v>
       </c>
       <c r="C36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D36">
         <v>4</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1111,12 +1222,15 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D37">
         <v>11</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modification de la bataille des cartes pour que le valet et neuf d'atout soit plus fort qu'un as d'atout. C'est un exemple
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
   <si>
     <t>Type</t>
   </si>
   <si>
-    <t>Valeur</t>
-  </si>
-  <si>
     <t>Valet</t>
   </si>
   <si>
@@ -172,6 +169,12 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>ValeurSansAtout</t>
+  </si>
+  <si>
+    <t>ValeurAvecAtout</t>
   </si>
 </sst>
 </file>
@@ -489,43 +492,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>6</v>
@@ -534,44 +540,50 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3">
-        <v>7</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -580,21 +592,24 @@
         <v>3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5">
         <v>9</v>
@@ -603,21 +618,24 @@
         <v>4</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>10</v>
@@ -626,113 +644,128 @@
         <v>5</v>
       </c>
       <c r="E6">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F10">
         <v>11</v>
       </c>
-      <c r="G10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>6</v>
@@ -741,21 +774,24 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>7</v>
@@ -764,21 +800,24 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -787,21 +826,24 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>9</v>
@@ -810,21 +852,24 @@
         <v>4</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>14</v>
       </c>
-      <c r="G14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>10</v>
@@ -833,113 +878,128 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
-      <c r="G15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16">
         <v>6</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
         <v>20</v>
       </c>
-      <c r="G16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
-      <c r="G17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>8</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F18">
         <v>4</v>
       </c>
-      <c r="G18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19">
         <v>9</v>
       </c>
       <c r="E19">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F19">
         <v>11</v>
       </c>
-      <c r="G19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>11</v>
+      </c>
+      <c r="H19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <v>6</v>
@@ -948,21 +1008,24 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -971,21 +1034,24 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -994,21 +1060,24 @@
         <v>3</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23">
         <v>9</v>
@@ -1017,21 +1086,24 @@
         <v>4</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
         <v>14</v>
       </c>
-      <c r="G23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24">
         <v>10</v>
@@ -1040,113 +1112,128 @@
         <v>5</v>
       </c>
       <c r="E24">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F24">
         <v>10</v>
       </c>
-      <c r="G24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>10</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>6</v>
       </c>
       <c r="E25">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F25">
+        <v>2</v>
+      </c>
+      <c r="G25">
         <v>20</v>
       </c>
-      <c r="G25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26">
         <v>7</v>
       </c>
       <c r="E26">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
-      <c r="G26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>3</v>
+      </c>
+      <c r="H26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27">
         <v>8</v>
       </c>
       <c r="E27">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
-      <c r="G27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
       <c r="E28">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F28">
         <v>11</v>
       </c>
-      <c r="G28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C29">
         <v>6</v>
@@ -1155,21 +1242,24 @@
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -1178,21 +1268,24 @@
         <v>2</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="G30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C31">
         <v>8</v>
@@ -1201,21 +1294,24 @@
         <v>3</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="G31" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32">
         <v>9</v>
@@ -1224,21 +1320,24 @@
         <v>4</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
         <v>14</v>
       </c>
-      <c r="G32" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C33">
         <v>10</v>
@@ -1247,105 +1346,120 @@
         <v>5</v>
       </c>
       <c r="E33">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="H33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <v>6</v>
       </c>
       <c r="E34">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="F34">
+        <v>2</v>
+      </c>
+      <c r="G34">
         <v>20</v>
       </c>
-      <c r="G34" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35">
         <v>7</v>
       </c>
       <c r="E35">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F35">
         <v>3</v>
       </c>
-      <c r="G35" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>3</v>
+      </c>
+      <c r="H35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D36">
         <v>8</v>
       </c>
       <c r="E36">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F36">
         <v>4</v>
       </c>
-      <c r="G36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>4</v>
+      </c>
+      <c r="H36" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D37">
         <v>9</v>
       </c>
       <c r="E37">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F37">
         <v>11</v>
       </c>
-      <c r="G37" t="s">
-        <v>47</v>
+      <c r="G37">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout d'une nouvelle règle et optimisation
</commit_message>
<xml_diff>
--- a/cards.xlsx
+++ b/cards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="51">
   <si>
     <t>Type</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>Coeur</t>
-  </si>
-  <si>
-    <t>Id</t>
   </si>
   <si>
     <t>ValeurSansAtout</t>
@@ -492,973 +489,862 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
         <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2">
-        <v>6</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
       <c r="C3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>48</v>
       </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
       <c r="C4">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>48</v>
       </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
       <c r="C5">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>14</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>48</v>
       </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
       <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
         <v>10</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
       </c>
       <c r="F6">
         <v>10</v>
       </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="G6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
       </c>
       <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>20</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
       <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-      <c r="H8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9">
         <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
-      <c r="G9">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10">
         <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
       </c>
       <c r="D10">
         <v>9</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>11</v>
       </c>
-      <c r="G10">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
       </c>
       <c r="C12">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D12">
         <v>2</v>
       </c>
       <c r="E12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>3</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
       </c>
       <c r="C14">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>14</v>
       </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>14</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
       </c>
       <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>5</v>
+      </c>
+      <c r="E15">
         <v>10</v>
-      </c>
-      <c r="D15">
-        <v>5</v>
-      </c>
-      <c r="E15">
-        <v>5</v>
       </c>
       <c r="F15">
         <v>10</v>
       </c>
-      <c r="G15">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
         <v>1</v>
       </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
       <c r="D16">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
         <v>20</v>
       </c>
-      <c r="F16">
-        <v>2</v>
-      </c>
-      <c r="G16">
-        <v>20</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="G16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
       <c r="E17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
-      <c r="G17">
-        <v>3</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="G17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
       </c>
       <c r="D18">
         <v>8</v>
       </c>
       <c r="E18">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F18">
         <v>4</v>
       </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>9</v>
       </c>
       <c r="D19">
         <v>9</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F19">
         <v>11</v>
       </c>
-      <c r="G19">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20">
         <v>6</v>
       </c>
       <c r="C20">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="G20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>6</v>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22">
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>6</v>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>14</v>
       </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>14</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>6</v>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
       </c>
       <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
         <v>10</v>
-      </c>
-      <c r="D24">
-        <v>5</v>
-      </c>
-      <c r="E24">
-        <v>5</v>
       </c>
       <c r="F24">
         <v>10</v>
       </c>
-      <c r="G24">
-        <v>10</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" t="s">
         <v>1</v>
       </c>
+      <c r="C25">
+        <v>6</v>
+      </c>
       <c r="D25">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
         <v>20</v>
       </c>
-      <c r="F25">
-        <v>2</v>
-      </c>
-      <c r="G25">
-        <v>20</v>
-      </c>
-      <c r="H25" t="s">
+      <c r="G25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>7</v>
       </c>
       <c r="D26">
         <v>7</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
-      <c r="G26">
-        <v>3</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="G26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
       </c>
       <c r="D27">
         <v>8</v>
       </c>
       <c r="E27">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F27">
         <v>4</v>
       </c>
-      <c r="G27">
-        <v>4</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>6</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C28">
+        <v>9</v>
       </c>
       <c r="D28">
         <v>9</v>
       </c>
       <c r="E28">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F28">
         <v>11</v>
       </c>
-      <c r="G28">
-        <v>11</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="G28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>7</v>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>6</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="G29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30">
         <v>7</v>
       </c>
       <c r="C30">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D30">
         <v>2</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>7</v>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>8</v>
       </c>
       <c r="C31">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D31">
         <v>3</v>
       </c>
       <c r="E31">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31" t="s">
+      <c r="G31" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <v>9</v>
       </c>
       <c r="C32">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D32">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>14</v>
       </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
-        <v>14</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="G32" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>7</v>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
       </c>
       <c r="C33">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
         <v>10</v>
-      </c>
-      <c r="D33">
-        <v>5</v>
-      </c>
-      <c r="E33">
-        <v>5</v>
       </c>
       <c r="F33">
         <v>10</v>
       </c>
-      <c r="G33">
-        <v>10</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="G33" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
         <v>1</v>
       </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
       <c r="D34">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
         <v>20</v>
       </c>
-      <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34">
-        <v>20</v>
-      </c>
-      <c r="H34" t="s">
+      <c r="G34" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>2</v>
+        <v>2</v>
+      </c>
+      <c r="C35">
+        <v>7</v>
       </c>
       <c r="D35">
         <v>7</v>
       </c>
       <c r="E35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F35">
         <v>3</v>
       </c>
-      <c r="G35">
-        <v>3</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="G35" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>8</v>
       </c>
       <c r="D36">
         <v>8</v>
       </c>
       <c r="E36">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F36">
         <v>4</v>
       </c>
-      <c r="G36">
-        <v>4</v>
-      </c>
-      <c r="H36" t="s">
+      <c r="G36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
-        <v>4</v>
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>9</v>
       </c>
       <c r="D37">
         <v>9</v>
       </c>
       <c r="E37">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F37">
         <v>11</v>
       </c>
-      <c r="G37">
-        <v>11</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="G37" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>